<commit_message>
created some commodity tsl cases; milestoneyear specification; unitconversion table in Syssettings.
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_New-CHP-DH.xlsx
+++ b/SubRES_TMPL/SubRES_New-CHP-DH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\DemoS_ADV_Stuttgart061118\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\Demo_Adv_Veda\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67026045-9FB7-44E0-99F7-FB449BCE1110}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF5B15D-065D-4DB9-9A41-8A863B84857D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELC_CHP" sheetId="9" r:id="rId1"/>
@@ -27,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,12 +37,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="I14" authorId="0" shapeId="0">
+    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -64,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J14" authorId="0" shapeId="0">
+    <comment ref="J15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -78,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I15" authorId="0" shapeId="0">
+    <comment ref="I16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -92,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J15" authorId="0" shapeId="0">
+    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -111,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="119">
   <si>
     <t>~FI_T</t>
   </si>
@@ -462,15 +464,21 @@
   </si>
   <si>
     <t>CAP2ACT</t>
+  </si>
+  <si>
+    <t>Residential heat from district heating network copy</t>
+  </si>
+  <si>
+    <t>SEASON</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="171" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="208" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="\Te\x\t"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -680,7 +688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -809,56 +817,56 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="208" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="208" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="208" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="208" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="208" fontId="13" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="208" fontId="13" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="208" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="208" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="208" fontId="3" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
-    <xf numFmtId="208" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="208" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="208" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="208" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="208" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="24">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
     <cellStyle name="Accent2" xfId="2" builtinId="33"/>
-    <cellStyle name="Comma 2" xfId="3"/>
+    <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="5"/>
-    <cellStyle name="Normal 2" xfId="6"/>
-    <cellStyle name="Normal 4" xfId="7"/>
-    <cellStyle name="Normal 4 2" xfId="8"/>
-    <cellStyle name="Normal 8" xfId="9"/>
-    <cellStyle name="Normal 9 2" xfId="10"/>
-    <cellStyle name="Normale_B2020" xfId="11"/>
-    <cellStyle name="Percent 2" xfId="12"/>
-    <cellStyle name="Percent 2 2" xfId="13"/>
-    <cellStyle name="Percent 3" xfId="14"/>
-    <cellStyle name="Percent 3 2" xfId="15"/>
-    <cellStyle name="Percent 4" xfId="16"/>
-    <cellStyle name="Percent 4 2" xfId="17"/>
-    <cellStyle name="Percent 5" xfId="18"/>
-    <cellStyle name="Percent 5 2" xfId="19"/>
-    <cellStyle name="Percent 5 3" xfId="20"/>
-    <cellStyle name="Percent 6" xfId="21"/>
-    <cellStyle name="Percent 7" xfId="22"/>
-    <cellStyle name="Standard_Sce_D_Extraction" xfId="23"/>
+    <cellStyle name="Normal 10" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 4 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 8" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 9 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normale_B2020" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Percent 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Percent 2 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Percent 3" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Percent 3 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Percent 4" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Percent 4 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Percent 5" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Percent 5 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Percent 5 3" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Percent 6" xfId="21" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Percent 7" xfId="22" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Standard_Sce_D_Extraction" xfId="23" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1328,10 +1336,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -2045,11 +2053,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2242,308 +2250,319 @@
         <v>56</v>
       </c>
       <c r="R8" s="67"/>
-      <c r="S8" s="67"/>
+      <c r="S8" s="67" t="s">
+        <v>112</v>
+      </c>
       <c r="T8" s="67"/>
       <c r="U8" s="67"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="L9" s="32"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
-      <c r="T9" s="31"/>
-      <c r="U9" s="31"/>
+      <c r="M9" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="N9" s="64"/>
+      <c r="O9" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="P9" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q9" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="R9" s="67"/>
+      <c r="S9" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="T9" s="67"/>
+      <c r="U9" s="67"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="D10" s="4" t="s">
+      <c r="L10" s="32"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="31"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="48"/>
-      <c r="M10" s="58" t="s">
+      <c r="E11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="48"/>
+      <c r="M11" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="N10" s="58"/>
-      <c r="O10" s="69"/>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="69"/>
-      <c r="R10" s="69"/>
-      <c r="S10" s="69"/>
-      <c r="T10" s="69"/>
-      <c r="U10" s="69"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B11" s="11" t="s">
+      <c r="N11" s="58"/>
+      <c r="O11" s="69"/>
+      <c r="P11" s="69"/>
+      <c r="Q11" s="69"/>
+      <c r="R11" s="69"/>
+      <c r="S11" s="69"/>
+      <c r="T11" s="69"/>
+      <c r="U11" s="69"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B12" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E12" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="56" t="s">
+      <c r="H12" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I12" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J12" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K12" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="M11" s="60" t="s">
+      <c r="M12" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="N11" s="61" t="s">
+      <c r="N12" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="O11" s="60" t="s">
+      <c r="O12" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="P11" s="60" t="s">
+      <c r="P12" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="Q11" s="60" t="s">
+      <c r="Q12" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="R11" s="60" t="s">
+      <c r="R12" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="S11" s="60" t="s">
+      <c r="S12" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="T11" s="60" t="s">
+      <c r="T12" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="U11" s="60" t="s">
+      <c r="U12" s="60" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="50" t="s">
+    <row r="13" spans="1:21" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C13" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D13" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15" t="s">
+      <c r="E13" s="15"/>
+      <c r="F13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G13" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="15" t="s">
+      <c r="H13" s="43"/>
+      <c r="I13" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="J13" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K13" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="M12" s="63" t="s">
+      <c r="M13" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="N12" s="63" t="s">
+      <c r="N13" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="O12" s="63" t="s">
+      <c r="O13" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="P12" s="63" t="s">
+      <c r="P13" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="Q12" s="63" t="s">
+      <c r="Q13" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="R12" s="63" t="s">
+      <c r="R13" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="S12" s="63" t="s">
+      <c r="S13" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="T12" s="63" t="s">
+      <c r="T13" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="U12" s="63" t="s">
+      <c r="U13" s="63" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="49" t="s">
+    <row r="14" spans="1:21" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="57" t="s">
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I14" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J14" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="K14" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="M13" s="63" t="s">
+      <c r="M14" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="N13" s="63"/>
-      <c r="O13" s="63"/>
-      <c r="P13" s="63"/>
-      <c r="Q13" s="63"/>
-      <c r="R13" s="63"/>
-      <c r="S13" s="63"/>
-      <c r="T13" s="63"/>
-      <c r="U13" s="63"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B14" s="39" t="str">
-        <f>O14</f>
+      <c r="N14" s="63"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="63"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
+      <c r="U14" s="63"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B15" s="39" t="str">
+        <f>O15</f>
         <v>RSHNHET1</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C15" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D15" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E15" s="38">
         <v>2015</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F15" s="37">
         <v>0.96</v>
       </c>
-      <c r="G14" s="36">
+      <c r="G15" s="36">
         <v>0.3</v>
       </c>
-      <c r="H14" s="35">
+      <c r="H15" s="35">
         <v>31.536000000000001</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I15" s="39">
         <v>250</v>
       </c>
-      <c r="J14" s="38">
+      <c r="J15" s="38">
         <v>5</v>
       </c>
-      <c r="K14" s="34">
+      <c r="K15" s="34">
         <v>20</v>
       </c>
-      <c r="M14" s="67" t="s">
+      <c r="M15" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="N14" s="69"/>
-      <c r="O14" s="67" t="s">
+      <c r="N15" s="69"/>
+      <c r="O15" s="67" t="s">
         <v>106</v>
       </c>
-      <c r="P14" s="70" t="s">
+      <c r="P15" s="70" t="s">
         <v>107</v>
-      </c>
-      <c r="Q14" s="64" t="s">
-        <v>56</v>
-      </c>
-      <c r="R14" s="64" t="s">
-        <v>57</v>
-      </c>
-      <c r="S14" s="69"/>
-      <c r="T14" s="69"/>
-      <c r="U14" s="69"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B15" s="44" t="str">
-        <f>O15</f>
-        <v>FTE-RSDHET</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" s="51">
-        <v>2015</v>
-      </c>
-      <c r="F15" s="52">
-        <v>0.95</v>
-      </c>
-      <c r="G15" s="42">
-        <v>1</v>
-      </c>
-      <c r="H15" s="6">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1000</v>
-      </c>
-      <c r="J15" s="51">
-        <v>10</v>
-      </c>
-      <c r="K15" s="32">
-        <v>20</v>
-      </c>
-      <c r="L15" s="55"/>
-      <c r="M15" s="69" t="s">
-        <v>96</v>
-      </c>
-      <c r="N15" s="69"/>
-      <c r="O15" s="64" t="s">
-        <v>109</v>
-      </c>
-      <c r="P15" s="71" t="s">
-        <v>108</v>
       </c>
       <c r="Q15" s="64" t="s">
         <v>56</v>
       </c>
       <c r="R15" s="64" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="S15" s="69"/>
       <c r="T15" s="69"/>
       <c r="U15" s="69"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
+      <c r="B16" s="44" t="str">
+        <f>O16</f>
+        <v>FTE-RSDHET</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="51">
+        <v>2015</v>
+      </c>
+      <c r="F16" s="52">
+        <v>0.95</v>
+      </c>
+      <c r="G16" s="42">
+        <v>1</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1000</v>
+      </c>
+      <c r="J16" s="51">
+        <v>10</v>
+      </c>
+      <c r="K16" s="32">
+        <v>20</v>
+      </c>
       <c r="L16" s="55"/>
+      <c r="M16" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="N16" s="69"/>
+      <c r="O16" s="64" t="s">
+        <v>109</v>
+      </c>
+      <c r="P16" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q16" s="64" t="s">
+        <v>56</v>
+      </c>
+      <c r="R16" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="S16" s="69"/>
+      <c r="T16" s="69"/>
+      <c r="U16" s="69"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="55"/>
@@ -2640,17 +2659,30 @@
       <c r="B24" s="55"/>
       <c r="C24" s="55"/>
       <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="28"/>
       <c r="J24" s="55"/>
       <c r="K24" s="55"/>
       <c r="L24" s="55"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B25" s="55"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
       <c r="L25" s="55"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L26" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>